<commit_message>
add particpant 4 study data
</commit_message>
<xml_diff>
--- a/StudyIDs.xlsx
+++ b/StudyIDs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pesek\SoftEngineering\SoftSpring2025\RegexStudy\Eye-Tracking-Study-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B28D9-FF2C-4E25-B918-5B8C13EA55DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA2C04C9-7256-4293-8CD1-C5001EEFED6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="3270" windowWidth="21600" windowHeight="11865" xr2:uid="{E20CAB67-0723-4A4F-8DA5-9A2D03268A2D}"/>
+    <workbookView xWindow="2565" yWindow="2025" windowWidth="21600" windowHeight="12645" xr2:uid="{E20CAB67-0723-4A4F-8DA5-9A2D03268A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Name</t>
   </si>
@@ -51,6 +51,9 @@
   </si>
   <si>
     <t>Eli Schone</t>
+  </si>
+  <si>
+    <t>Grey Nclayghlin</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -467,6 +470,9 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
       <c r="B5">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Added information from questionaires
</commit_message>
<xml_diff>
--- a/StudyIDs.xlsx
+++ b/StudyIDs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pesek\SoftEngineering\SoftSpring2025\RegexStudy\Eye-Tracking-Study-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{055B3F68-7C64-40FC-AFD9-54223BDB85DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B8D0FF0-193C-44F1-96DE-FF21C5248134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="12645" xr2:uid="{E20CAB67-0723-4A4F-8DA5-9A2D03268A2D}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{E20CAB67-0723-4A4F-8DA5-9A2D03268A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>??</t>
+  </si>
+  <si>
+    <t>Rachel Solberg</t>
   </si>
 </sst>
 </file>
@@ -434,7 +437,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,6 +503,9 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
       <c r="B8">
         <v>7</v>
       </c>

</xml_diff>